<commit_message>
correcciones de sergio (3)
</commit_message>
<xml_diff>
--- a/Repositorio/Proyecto/DocumentosPropios/GrpL_MGI_181018_MatrizGestionInteresados_v1.xlsx
+++ b/Repositorio/Proyecto/DocumentosPropios/GrpL_MGI_181018_MatrizGestionInteresados_v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\USC\Cuarto\XesPro\Proxecto\7\Vainas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergy6rey\Documents\GitHub\PracticaXesPro_GrupoL\Repositorio\Proyecto\DocumentosPropios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310A51C7-3C1F-4860-A291-983575759F1B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85CF11F-0156-4ADA-93C3-A9FDE4C86B14}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="108">
   <si>
     <t>Nombre</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>Miembro de equipo de proyecto</t>
-  </si>
-  <si>
-    <t>Analista</t>
   </si>
   <si>
     <t>Patrocinador y máximo dirigente</t>
@@ -366,6 +363,21 @@
   </si>
   <si>
     <t>Reunión presencial y WhatsApp</t>
+  </si>
+  <si>
+    <t>Abogado GEI SOFT</t>
+  </si>
+  <si>
+    <t>Abogado EjoSL</t>
+  </si>
+  <si>
+    <t>Representante legal de GEI SOFT</t>
+  </si>
+  <si>
+    <t>Representante legal de EjoSL</t>
+  </si>
+  <si>
+    <t>Comunicación con el equipo.</t>
   </si>
 </sst>
 </file>
@@ -591,7 +603,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Texto explicativo" xfId="2" builtinId="53"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1032,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F7"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,13 +1090,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1075,16 +1107,16 @@
         <v>36</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1095,10 +1127,10 @@
         <v>37</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
@@ -1111,10 +1143,10 @@
         <v>37</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
@@ -1127,10 +1159,10 @@
         <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -1140,13 +1172,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -1156,13 +1188,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -1172,19 +1204,19 @@
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -1192,19 +1224,19 @@
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="89.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1212,19 +1244,19 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1232,19 +1264,19 @@
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -1252,19 +1284,19 @@
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -1272,19 +1304,19 @@
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1292,19 +1324,19 @@
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1312,19 +1344,19 @@
         <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1332,13 +1364,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
@@ -1348,13 +1380,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="14"/>
@@ -1364,13 +1396,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -1380,19 +1412,19 @@
         <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1400,19 +1432,19 @@
         <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="E20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1420,19 +1452,19 @@
         <v>23</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1443,10 +1475,10 @@
         <v>24</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -1456,19 +1488,19 @@
         <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1476,19 +1508,19 @@
         <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1496,19 +1528,19 @@
         <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="E25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1516,19 +1548,19 @@
         <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1536,19 +1568,19 @@
         <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1556,19 +1588,19 @@
         <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1576,19 +1608,19 @@
         <v>31</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="E29" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1596,19 +1628,19 @@
         <v>32</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1616,19 +1648,19 @@
         <v>33</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1636,19 +1668,19 @@
         <v>34</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="E32" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1656,19 +1688,59 @@
         <v>35</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +1753,52 @@
     <mergeCell ref="F21:F22"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="12" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="27" operator="equal">
+      <formula>"ALTO"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="13" priority="29" operator="equal">
+      <formula>"ALTO"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="cellIs" dxfId="12" priority="25" operator="equal">
+      <formula>"ALTO"</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="11" priority="23" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="24">
@@ -1695,22 +1812,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="11" priority="25" operator="equal">
-      <formula>"ALTO"</formula>
-    </cfRule>
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
+  <conditionalFormatting sqref="C19">
     <cfRule type="cellIs" dxfId="10" priority="21" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -1725,7 +1827,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
+  <conditionalFormatting sqref="C24">
     <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -1740,7 +1842,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
+  <conditionalFormatting sqref="D2">
     <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -1755,7 +1857,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
+  <conditionalFormatting sqref="D8">
     <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -1770,7 +1872,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D3">
     <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -1785,7 +1887,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+  <conditionalFormatting sqref="D4">
     <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -1800,7 +1902,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
+  <conditionalFormatting sqref="D5">
     <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -1815,7 +1917,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
+  <conditionalFormatting sqref="D10">
     <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -1830,7 +1932,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
+  <conditionalFormatting sqref="D11">
     <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -1845,7 +1947,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
+  <conditionalFormatting sqref="D34">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>
@@ -1860,7 +1962,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
+  <conditionalFormatting sqref="D35">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"ALTO"</formula>
     </cfRule>

</xml_diff>